<commit_message>
propuesta de fase 2
</commit_message>
<xml_diff>
--- a/docs/RESPUESTAS MOD. LIQ.xlsx
+++ b/docs/RESPUESTAS MOD. LIQ.xlsx
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>